<commit_message>
integration tests now passing... onwards!
</commit_message>
<xml_diff>
--- a/modules/lib-excel/integtests/src/test/resources/org/incode/platform/lib/excel/integtests/tests/ToDoItemsWithMultipleSheets.xlsx
+++ b/modules/lib-excel/integtests/src/test/resources/org/incode/platform/lib/excel/integtests/tests/ToDoItemsWithMultipleSheets.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvanderwal/src/github/isisaddons/isis-module-excel/integtests/src/test/java/org/isisaddons/module/excel/integtests/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\incodehq\incode-platform\modules\lib-excel\integtests\src\test\resources\org\incode\platform\lib\excel\integtests\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="24960" windowHeight="13480"/>
+    <workbookView xWindow="480" yWindow="465" windowWidth="24960" windowHeight="13485"/>
   </bookViews>
   <sheets>
-    <sheet name="ExcelModuleDemoToDoItem" sheetId="1" r:id="rId1"/>
-    <sheet name="ExcelModuleDemoProfessionalImp" sheetId="4" r:id="rId2"/>
+    <sheet name="DemoToDoItem" sheetId="1" r:id="rId1"/>
+    <sheet name="ExcelUploadRowHandler4ToDoItem" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -107,8 +107,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,16 +486,16 @@
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -515,7 +515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -535,7 +535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="C3" t="s">
         <v>5</v>
@@ -550,7 +550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="C4" t="s">
         <v>6</v>
@@ -562,7 +562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>13</v>
@@ -577,7 +577,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>14</v>
@@ -589,7 +589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>15</v>
@@ -601,7 +601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>13</v>
@@ -613,19 +613,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
@@ -645,16 +645,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -674,7 +674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -706,7 +706,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -718,7 +718,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>